<commit_message>
feat: run other algorithms
</commit_message>
<xml_diff>
--- a/results/evaluation_chd_49_noisy_0.0_clr.xlsx
+++ b/results/evaluation_chd_49_noisy_0.0_clr.xlsx
@@ -31,7 +31,7 @@
     <t>Std</t>
   </si>
   <si>
-    <t>RF</t>
+    <t>LightGBM</t>
   </si>
   <si>
     <t>CLR</t>
@@ -435,10 +435,10 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0.68319</v>
+        <v>0.67237</v>
       </c>
       <c r="E2">
-        <v>0.00213</v>
+        <v>0.00091</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -452,10 +452,10 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>0.08287</v>
+        <v>0.09369</v>
       </c>
       <c r="E3">
-        <v>0.00706</v>
+        <v>0.00017</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -469,10 +469,10 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>0.49528</v>
+        <v>0.5017200000000001</v>
       </c>
       <c r="E4">
-        <v>0.01247</v>
+        <v>0.00061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>